<commit_message>
Adicionando script que será usado para gerar gráficos para o relatório/artigo
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/Comparações dos valores de m para o graspRVND Semi-aleatório.xlsx
+++ b/Arquivos/Comparações/Comparações dos valores de m para o graspRVND Semi-aleatório.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885"/>
+    <workbookView windowWidth="28785" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -171,15 +171,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0_ "/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -200,26 +207,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -240,7 +247,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,47 +283,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,15 +300,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,10 +320,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -352,13 +359,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,25 +401,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,13 +443,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,103 +515,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,6 +534,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,6 +568,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -572,6 +590,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,6 +618,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -602,24 +638,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,168 +665,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -844,6 +851,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1178,8 +1188,8 @@
   <sheetPr/>
   <dimension ref="C3:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:Q48"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1349,13 +1359,21 @@
       <c r="T5" s="11">
         <v>210</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="10" t="e">
+      <c r="U5" s="4">
+        <v>1868.43</v>
+      </c>
+      <c r="V5" s="4">
+        <v>1865.42</v>
+      </c>
+      <c r="W5" s="4">
+        <v>1885.73</v>
+      </c>
+      <c r="X5" s="12">
+        <v>1892.27</v>
+      </c>
+      <c r="Y5" s="10">
         <f>SMALL(U5:X5,1)</f>
-        <v>#NUM!</v>
+        <v>1865.42</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="3:25">
@@ -1409,13 +1427,21 @@
       <c r="T6" s="11">
         <v>21</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="10" t="e">
+      <c r="U6" s="4">
+        <v>918</v>
+      </c>
+      <c r="V6" s="4">
+        <v>918</v>
+      </c>
+      <c r="W6" s="4">
+        <v>918</v>
+      </c>
+      <c r="X6" s="12">
+        <v>918</v>
+      </c>
+      <c r="Y6" s="10">
         <f t="shared" ref="Y6:Y48" si="2">SMALL(U6:X6,1)</f>
-        <v>#NUM!</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="3:25">
@@ -1469,13 +1495,21 @@
       <c r="T7" s="11">
         <v>21</v>
       </c>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="10" t="e">
+      <c r="U7" s="4">
+        <v>1086</v>
+      </c>
+      <c r="V7" s="4">
+        <v>1086</v>
+      </c>
+      <c r="W7" s="4">
+        <v>1086</v>
+      </c>
+      <c r="X7" s="12">
+        <v>1086</v>
+      </c>
+      <c r="Y7" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="3:25">
@@ -1529,13 +1563,21 @@
       <c r="T8" s="11">
         <v>39</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="10" t="e">
+      <c r="U8" s="4">
+        <v>3853.08</v>
+      </c>
+      <c r="V8" s="4">
+        <v>3853.08</v>
+      </c>
+      <c r="W8" s="4">
+        <v>3855.72</v>
+      </c>
+      <c r="X8" s="12">
+        <v>3853.08</v>
+      </c>
+      <c r="Y8" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>3853.08</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="3:25">
@@ -1589,13 +1631,21 @@
       <c r="T9" s="11">
         <v>95</v>
       </c>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="10" t="e">
+      <c r="U9" s="4">
+        <v>48894.04</v>
+      </c>
+      <c r="V9" s="4">
+        <v>48293.73</v>
+      </c>
+      <c r="W9" s="4">
+        <v>48840.78</v>
+      </c>
+      <c r="X9" s="12">
+        <v>49010.93</v>
+      </c>
+      <c r="Y9" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>48293.73</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="3:25">
@@ -1649,13 +1699,21 @@
       <c r="T10" s="11">
         <v>10</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="10" t="e">
+      <c r="U10" s="4">
+        <v>1528.5</v>
+      </c>
+      <c r="V10" s="4">
+        <v>1528.5</v>
+      </c>
+      <c r="W10" s="4">
+        <v>1528.5</v>
+      </c>
+      <c r="X10" s="12">
+        <v>1528.5</v>
+      </c>
+      <c r="Y10" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1528.5</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="3:25">
@@ -1709,13 +1767,21 @@
       <c r="T11" s="11">
         <v>97</v>
       </c>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="10" t="e">
+      <c r="U11" s="4">
+        <v>3805.85</v>
+      </c>
+      <c r="V11" s="4">
+        <v>3776.77</v>
+      </c>
+      <c r="W11" s="4">
+        <v>3783.8</v>
+      </c>
+      <c r="X11" s="12">
+        <v>3786.09</v>
+      </c>
+      <c r="Y11" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>3776.77</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="3:25">
@@ -1769,13 +1835,21 @@
       <c r="T12" s="11">
         <v>112</v>
       </c>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="10" t="e">
+      <c r="U12" s="4">
+        <v>4239.49</v>
+      </c>
+      <c r="V12" s="4">
+        <v>4263.84</v>
+      </c>
+      <c r="W12" s="4">
+        <v>4316.09</v>
+      </c>
+      <c r="X12" s="12">
+        <v>4257.66</v>
+      </c>
+      <c r="Y12" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>4239.49</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="3:25">
@@ -1829,13 +1903,21 @@
       <c r="T13" s="11">
         <v>31</v>
       </c>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="10" t="e">
+      <c r="U13" s="4">
+        <v>389</v>
+      </c>
+      <c r="V13" s="4">
+        <v>388</v>
+      </c>
+      <c r="W13" s="4">
+        <v>388</v>
+      </c>
+      <c r="X13" s="12">
+        <v>388</v>
+      </c>
+      <c r="Y13" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="3:25">
@@ -1889,13 +1971,21 @@
       <c r="T14" s="11">
         <v>38</v>
       </c>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="10" t="e">
+      <c r="U14" s="4">
+        <v>272.79</v>
+      </c>
+      <c r="V14" s="4">
+        <v>272.79</v>
+      </c>
+      <c r="W14" s="4">
+        <v>272.79</v>
+      </c>
+      <c r="X14" s="12">
+        <v>272.79</v>
+      </c>
+      <c r="Y14" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>272.79</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="3:25">
@@ -1949,13 +2039,21 @@
       <c r="T15" s="11">
         <v>57</v>
       </c>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="10" t="e">
+      <c r="U15" s="4">
+        <v>334.89</v>
+      </c>
+      <c r="V15" s="4">
+        <v>336.47</v>
+      </c>
+      <c r="W15" s="4">
+        <v>340.02</v>
+      </c>
+      <c r="X15" s="12">
+        <v>338.57</v>
+      </c>
+      <c r="Y15" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>334.89</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="3:25">
@@ -2009,13 +2107,21 @@
       <c r="T16" s="11">
         <v>75</v>
       </c>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="10" t="e">
+      <c r="U16" s="4">
+        <v>387.72</v>
+      </c>
+      <c r="V16" s="4">
+        <v>386.68</v>
+      </c>
+      <c r="W16" s="4">
+        <v>387.51</v>
+      </c>
+      <c r="X16" s="12">
+        <v>387.72</v>
+      </c>
+      <c r="Y16" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>386.68</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="3:25">
@@ -2069,13 +2175,21 @@
       <c r="T17" s="11">
         <v>19</v>
       </c>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="10" t="e">
+      <c r="U17" s="4">
+        <v>492</v>
+      </c>
+      <c r="V17" s="4">
+        <v>492</v>
+      </c>
+      <c r="W17" s="4">
+        <v>492</v>
+      </c>
+      <c r="X17" s="12">
+        <v>492</v>
+      </c>
+      <c r="Y17" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" ht="15.75" spans="3:25">
@@ -2129,13 +2243,21 @@
       <c r="T18" s="11">
         <v>196</v>
       </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="10" t="e">
+      <c r="U18" s="4">
+        <v>1585.88</v>
+      </c>
+      <c r="V18" s="4">
+        <v>1576.44</v>
+      </c>
+      <c r="W18" s="4">
+        <v>1577.96</v>
+      </c>
+      <c r="X18" s="12">
+        <v>1578.98</v>
+      </c>
+      <c r="Y18" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1576.44</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="3:25">
@@ -2189,13 +2311,21 @@
       <c r="T19" s="11">
         <v>12</v>
       </c>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="10" t="e">
+      <c r="U19" s="4">
+        <v>640</v>
+      </c>
+      <c r="V19" s="4">
+        <v>640</v>
+      </c>
+      <c r="W19" s="4">
+        <v>640</v>
+      </c>
+      <c r="X19" s="12">
+        <v>640</v>
+      </c>
+      <c r="Y19" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="3:25">
@@ -2249,13 +2379,21 @@
       <c r="T20" s="11">
         <v>15</v>
       </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="10" t="e">
+      <c r="U20" s="4">
+        <v>1276</v>
+      </c>
+      <c r="V20" s="4">
+        <v>1276</v>
+      </c>
+      <c r="W20" s="4">
+        <v>1276</v>
+      </c>
+      <c r="X20" s="12">
+        <v>1276</v>
+      </c>
+      <c r="Y20" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="3:25">
@@ -2309,13 +2447,21 @@
       <c r="T21" s="11">
         <v>18</v>
       </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="10" t="e">
+      <c r="U21" s="4">
+        <v>748</v>
+      </c>
+      <c r="V21" s="4">
+        <v>748</v>
+      </c>
+      <c r="W21" s="4">
+        <v>748</v>
+      </c>
+      <c r="X21" s="12">
+        <v>748</v>
+      </c>
+      <c r="Y21" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>748</v>
       </c>
     </row>
     <row r="22" ht="15.75" spans="3:25">
@@ -2369,13 +2515,21 @@
       <c r="T22" s="11">
         <v>36</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="10" t="e">
+      <c r="U22" s="4">
+        <v>2909</v>
+      </c>
+      <c r="V22" s="4">
+        <v>2909</v>
+      </c>
+      <c r="W22" s="4">
+        <v>2926</v>
+      </c>
+      <c r="X22" s="12">
+        <v>2909</v>
+      </c>
+      <c r="Y22" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="3:25">
@@ -2429,13 +2583,21 @@
       <c r="T23" s="11">
         <v>72</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="10" t="e">
+      <c r="U23" s="4">
+        <v>32229.45</v>
+      </c>
+      <c r="V23" s="4">
+        <v>32191.47</v>
+      </c>
+      <c r="W23" s="4">
+        <v>32228.83</v>
+      </c>
+      <c r="X23" s="12">
+        <v>32267.14</v>
+      </c>
+      <c r="Y23" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>32191.47</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="3:25">
@@ -2489,13 +2651,21 @@
       <c r="T24" s="11">
         <v>36</v>
       </c>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="10" t="e">
+      <c r="U24" s="4">
+        <v>6858</v>
+      </c>
+      <c r="V24" s="4">
+        <v>6866</v>
+      </c>
+      <c r="W24" s="4">
+        <v>6838</v>
+      </c>
+      <c r="X24" s="12">
+        <v>6814</v>
+      </c>
+      <c r="Y24" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>6814</v>
       </c>
     </row>
     <row r="25" ht="15.75" spans="3:25">
@@ -2549,13 +2719,21 @@
       <c r="T25" s="11">
         <v>75</v>
       </c>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="10" t="e">
+      <c r="U25" s="4">
+        <v>14178.1</v>
+      </c>
+      <c r="V25" s="4">
+        <v>13974.03</v>
+      </c>
+      <c r="W25" s="4">
+        <v>13912.79</v>
+      </c>
+      <c r="X25" s="12">
+        <v>14146.57</v>
+      </c>
+      <c r="Y25" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>13912.79</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="3:25">
@@ -2609,13 +2787,21 @@
       <c r="T26" s="11">
         <v>112</v>
       </c>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="10" t="e">
+      <c r="U26" s="4">
+        <v>17143.7</v>
+      </c>
+      <c r="V26" s="4">
+        <v>17475.99</v>
+      </c>
+      <c r="W26" s="4">
+        <v>17385.59</v>
+      </c>
+      <c r="X26" s="12">
+        <v>17502.18</v>
+      </c>
+      <c r="Y26" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>17143.7</v>
       </c>
     </row>
     <row r="27" ht="15.75" spans="3:25">
@@ -2669,13 +2855,21 @@
       <c r="T27" s="11">
         <v>150</v>
       </c>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="10" t="e">
+      <c r="U27" s="4">
+        <v>19790.72</v>
+      </c>
+      <c r="V27" s="4">
+        <v>19529.8</v>
+      </c>
+      <c r="W27" s="4">
+        <v>19541.15</v>
+      </c>
+      <c r="X27" s="12">
+        <v>19620.35</v>
+      </c>
+      <c r="Y27" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>19529.8</v>
       </c>
     </row>
     <row r="28" ht="15.75" spans="3:25">
@@ -2729,13 +2923,21 @@
       <c r="T28" s="11">
         <v>75</v>
       </c>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="10" t="e">
+      <c r="U28" s="4">
+        <v>13951.96</v>
+      </c>
+      <c r="V28" s="4">
+        <v>14094.71</v>
+      </c>
+      <c r="W28" s="4">
+        <v>14115.73</v>
+      </c>
+      <c r="X28" s="12">
+        <v>14119.56</v>
+      </c>
+      <c r="Y28" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>13951.96</v>
       </c>
     </row>
     <row r="29" ht="15.75" spans="3:25">
@@ -2789,13 +2991,21 @@
       <c r="T29" s="11">
         <v>112</v>
       </c>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="10" t="e">
+      <c r="U29" s="4">
+        <v>16489.24</v>
+      </c>
+      <c r="V29" s="4">
+        <v>16599.04</v>
+      </c>
+      <c r="W29" s="4">
+        <v>16556.09</v>
+      </c>
+      <c r="X29" s="12">
+        <v>16617.16</v>
+      </c>
+      <c r="Y29" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>16489.24</v>
       </c>
     </row>
     <row r="30" ht="15.75" spans="3:25">
@@ -2849,13 +3059,21 @@
       <c r="T30" s="11">
         <v>150</v>
       </c>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="10" t="e">
+      <c r="U30" s="4">
+        <v>19679.39</v>
+      </c>
+      <c r="V30" s="4">
+        <v>19872.76</v>
+      </c>
+      <c r="W30" s="4">
+        <v>19560.77</v>
+      </c>
+      <c r="X30" s="12">
+        <v>19701.02</v>
+      </c>
+      <c r="Y30" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>19560.77</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="3:25">
@@ -2909,13 +3127,21 @@
       <c r="T31" s="11">
         <v>75</v>
       </c>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="10" t="e">
+      <c r="U31" s="4">
+        <v>13368.28</v>
+      </c>
+      <c r="V31" s="4">
+        <v>13347.5</v>
+      </c>
+      <c r="W31" s="4">
+        <v>13415.64</v>
+      </c>
+      <c r="X31" s="12">
+        <v>13198.92</v>
+      </c>
+      <c r="Y31" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>13198.92</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="3:25">
@@ -2969,13 +3195,21 @@
       <c r="T32" s="11">
         <v>75</v>
       </c>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="10" t="e">
+      <c r="U32" s="4">
+        <v>14096.41</v>
+      </c>
+      <c r="V32" s="4">
+        <v>14097.28</v>
+      </c>
+      <c r="W32" s="4">
+        <v>14072.63</v>
+      </c>
+      <c r="X32" s="12">
+        <v>13939.71</v>
+      </c>
+      <c r="Y32" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>13939.71</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="3:25">
@@ -3029,13 +3263,21 @@
       <c r="T33" s="11">
         <v>75</v>
       </c>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="10" t="e">
+      <c r="U33" s="4">
+        <v>14388.46</v>
+      </c>
+      <c r="V33" s="4">
+        <v>14383.86</v>
+      </c>
+      <c r="W33" s="4">
+        <v>14397.84</v>
+      </c>
+      <c r="X33" s="12">
+        <v>14528.75</v>
+      </c>
+      <c r="Y33" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>14383.86</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="3:25">
@@ -3089,13 +3331,21 @@
       <c r="T34" s="11">
         <v>78</v>
       </c>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="10" t="e">
+      <c r="U34" s="4">
+        <v>7785.16</v>
+      </c>
+      <c r="V34" s="4">
+        <v>7787.21</v>
+      </c>
+      <c r="W34" s="4">
+        <v>7787.21</v>
+      </c>
+      <c r="X34" s="12">
+        <v>7754.43</v>
+      </c>
+      <c r="Y34" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>7754.43</v>
       </c>
     </row>
     <row r="35" ht="15.75" spans="3:25">
@@ -3149,13 +3399,21 @@
       <c r="T35" s="11">
         <v>238</v>
       </c>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="10" t="e">
+      <c r="U35" s="4">
+        <v>26477.62</v>
+      </c>
+      <c r="V35" s="4">
+        <v>26382.45</v>
+      </c>
+      <c r="W35" s="4">
+        <v>25818.91</v>
+      </c>
+      <c r="X35" s="12">
+        <v>25735.51</v>
+      </c>
+      <c r="Y35" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>25735.51</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="3:25">
@@ -3209,13 +3467,21 @@
       <c r="T36" s="11">
         <v>57</v>
       </c>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="10" t="e">
+      <c r="U36" s="4">
+        <v>59775.72</v>
+      </c>
+      <c r="V36" s="4">
+        <v>59615.43</v>
+      </c>
+      <c r="W36" s="4">
+        <v>59799.67</v>
+      </c>
+      <c r="X36" s="12">
+        <v>59497.82</v>
+      </c>
+      <c r="Y36" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>59497.82</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="3:25">
@@ -3269,13 +3535,21 @@
       <c r="T37" s="11">
         <v>80</v>
       </c>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="10" t="e">
+      <c r="U37" s="4">
+        <v>29241.06</v>
+      </c>
+      <c r="V37" s="4">
+        <v>29402.34</v>
+      </c>
+      <c r="W37" s="4">
+        <v>29309.69</v>
+      </c>
+      <c r="X37" s="12">
+        <v>29402.34</v>
+      </c>
+      <c r="Y37" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>29241.06</v>
       </c>
     </row>
     <row r="38" ht="15.75" spans="3:25">
@@ -3329,13 +3603,21 @@
       <c r="T38" s="11">
         <v>93</v>
       </c>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="10" t="e">
+      <c r="U38" s="4">
+        <v>35368.11</v>
+      </c>
+      <c r="V38" s="4">
+        <v>35368.11</v>
+      </c>
+      <c r="W38" s="4">
+        <v>35356.08</v>
+      </c>
+      <c r="X38" s="12">
+        <v>35356.08</v>
+      </c>
+      <c r="Y38" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>35356.08</v>
       </c>
     </row>
     <row r="39" ht="15.75" spans="3:25">
@@ -3389,13 +3671,21 @@
       <c r="T39" s="11">
         <v>102</v>
       </c>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="10" t="e">
+      <c r="U39" s="4">
+        <v>66037.14</v>
+      </c>
+      <c r="V39" s="4">
+        <v>65647.42</v>
+      </c>
+      <c r="W39" s="4">
+        <v>65889.36</v>
+      </c>
+      <c r="X39" s="12">
+        <v>65395.56</v>
+      </c>
+      <c r="Y39" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>65395.56</v>
       </c>
     </row>
     <row r="40" ht="15.75" spans="3:25">
@@ -3449,13 +3739,21 @@
       <c r="T40" s="11">
         <v>108</v>
       </c>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="10" t="e">
+      <c r="U40" s="4">
+        <v>38851.86</v>
+      </c>
+      <c r="V40" s="4">
+        <v>38892.59</v>
+      </c>
+      <c r="W40" s="4">
+        <v>38892.59</v>
+      </c>
+      <c r="X40" s="12">
+        <v>39254.32</v>
+      </c>
+      <c r="Y40" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>38851.86</v>
       </c>
     </row>
     <row r="41" ht="15.75" spans="3:25">
@@ -3509,13 +3807,21 @@
       <c r="T41" s="11">
         <v>114</v>
       </c>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="10" t="e">
+      <c r="U41" s="4">
+        <v>45889.61</v>
+      </c>
+      <c r="V41" s="4">
+        <v>45878.65</v>
+      </c>
+      <c r="W41" s="4">
+        <v>45878.65</v>
+      </c>
+      <c r="X41" s="12">
+        <v>45878.65</v>
+      </c>
+      <c r="Y41" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>45878.65</v>
       </c>
     </row>
     <row r="42" ht="15.75" spans="3:25">
@@ -3569,13 +3875,21 @@
       <c r="T42" s="11">
         <v>169</v>
       </c>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="4"/>
-      <c r="Y42" s="10" t="e">
+      <c r="U42" s="4">
+        <v>46002.48</v>
+      </c>
+      <c r="V42" s="4">
+        <v>45999.44</v>
+      </c>
+      <c r="W42" s="4">
+        <v>45965.05</v>
+      </c>
+      <c r="X42" s="12">
+        <v>46036.72</v>
+      </c>
+      <c r="Y42" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>45965.05</v>
       </c>
     </row>
     <row r="43" ht="15.75" spans="3:25">
@@ -3629,13 +3943,21 @@
       <c r="T43" s="11">
         <v>74</v>
       </c>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
-      <c r="X43" s="4"/>
-      <c r="Y43" s="10" t="e">
+      <c r="U43" s="4">
+        <v>835.08</v>
+      </c>
+      <c r="V43" s="4">
+        <v>836.57</v>
+      </c>
+      <c r="W43" s="4">
+        <v>839.91</v>
+      </c>
+      <c r="X43" s="12">
+        <v>841.45</v>
+      </c>
+      <c r="Y43" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>835.08</v>
       </c>
     </row>
     <row r="44" ht="15.75" spans="3:25">
@@ -3689,13 +4011,21 @@
       <c r="T44" s="11">
         <v>146</v>
       </c>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="4"/>
-      <c r="Y44" s="10" t="e">
+      <c r="U44" s="4">
+        <v>1666.98</v>
+      </c>
+      <c r="V44" s="4">
+        <v>1666.72</v>
+      </c>
+      <c r="W44" s="4">
+        <v>1657.94</v>
+      </c>
+      <c r="X44" s="12">
+        <v>1663.58</v>
+      </c>
+      <c r="Y44" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1657.94</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="3:25">
@@ -3749,13 +4079,21 @@
       <c r="T45" s="11">
         <v>52</v>
       </c>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="4"/>
-      <c r="Y45" s="10" t="e">
+      <c r="U45" s="4">
+        <v>421.18</v>
+      </c>
+      <c r="V45" s="4">
+        <v>421.18</v>
+      </c>
+      <c r="W45" s="4">
+        <v>418.08</v>
+      </c>
+      <c r="X45" s="12">
+        <v>421.18</v>
+      </c>
+      <c r="Y45" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>418.08</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="3:25">
@@ -3809,13 +4147,21 @@
       <c r="T46" s="11">
         <v>31</v>
       </c>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
-      <c r="W46" s="4"/>
-      <c r="X46" s="4"/>
-      <c r="Y46" s="10" t="e">
+      <c r="U46" s="4">
+        <v>698</v>
+      </c>
+      <c r="V46" s="4">
+        <v>698</v>
+      </c>
+      <c r="W46" s="4">
+        <v>698</v>
+      </c>
+      <c r="X46" s="12">
+        <v>698</v>
+      </c>
+      <c r="Y46" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>698</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="3:25">
@@ -3869,13 +4215,21 @@
       <c r="T47" s="11">
         <v>12</v>
       </c>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="10" t="e">
+      <c r="U47" s="4">
+        <v>2731</v>
+      </c>
+      <c r="V47" s="4">
+        <v>2731</v>
+      </c>
+      <c r="W47" s="4">
+        <v>2731</v>
+      </c>
+      <c r="X47" s="12">
+        <v>2731</v>
+      </c>
+      <c r="Y47" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="48" ht="15.75" spans="3:25">
@@ -3929,13 +4283,21 @@
       <c r="T48" s="11">
         <v>16</v>
       </c>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="10" t="e">
+      <c r="U48" s="4">
+        <v>2540.07</v>
+      </c>
+      <c r="V48" s="4">
+        <v>2540.07</v>
+      </c>
+      <c r="W48" s="4">
+        <v>2540.07</v>
+      </c>
+      <c r="X48" s="12">
+        <v>2540.07</v>
+      </c>
+      <c r="Y48" s="10">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>2540.07</v>
       </c>
     </row>
     <row r="49" spans="3:24">

</xml_diff>